<commit_message>
Added colors by values of temp. and hum. in PDF
</commit_message>
<xml_diff>
--- a/SensorMessungen.xlsx
+++ b/SensorMessungen.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G426"/>
+  <dimension ref="A1:G484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13642,6 +13642,1804 @@
         </is>
       </c>
     </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>426</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>12:30:19</t>
+        </is>
+      </c>
+      <c r="D427" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="E427" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>0.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>427</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>12:31:25</t>
+        </is>
+      </c>
+      <c r="D428" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="E428" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>428</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>12:32:27</t>
+        </is>
+      </c>
+      <c r="D429" t="n">
+        <v>32</v>
+      </c>
+      <c r="E429" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>429</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>12:54:30</t>
+        </is>
+      </c>
+      <c r="D430" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="E430" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="F430" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>430</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>12:55:27</t>
+        </is>
+      </c>
+      <c r="D431" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E431" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="F431" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>431</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>12:56:48</t>
+        </is>
+      </c>
+      <c r="D432" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="E432" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>432</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>13:01:12</t>
+        </is>
+      </c>
+      <c r="D433" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="E433" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>433</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>13:03:18</t>
+        </is>
+      </c>
+      <c r="D434" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="E434" t="n">
+        <v>21</v>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>434</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>13:04:41</t>
+        </is>
+      </c>
+      <c r="D435" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="E435" t="n">
+        <v>21</v>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>435</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>13:05:42</t>
+        </is>
+      </c>
+      <c r="D436" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="E436" t="n">
+        <v>21</v>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>436</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>13:06:19</t>
+        </is>
+      </c>
+      <c r="D437" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E437" t="n">
+        <v>21</v>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>437</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>13:09:33</t>
+        </is>
+      </c>
+      <c r="D438" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E438" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>438</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>13:34:56</t>
+        </is>
+      </c>
+      <c r="D439" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="E439" t="n">
+        <v>21</v>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>439</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>13:36:01</t>
+        </is>
+      </c>
+      <c r="D440" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E440" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>440</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>13:37:05</t>
+        </is>
+      </c>
+      <c r="D441" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E441" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>441</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>13:38:06</t>
+        </is>
+      </c>
+      <c r="D442" t="n">
+        <v>34</v>
+      </c>
+      <c r="E442" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>442</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>13:39:10</t>
+        </is>
+      </c>
+      <c r="D443" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E443" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>443</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>13:40:39</t>
+        </is>
+      </c>
+      <c r="D444" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E444" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>444</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>13:41:47</t>
+        </is>
+      </c>
+      <c r="D445" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E445" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>445</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>13:42:48</t>
+        </is>
+      </c>
+      <c r="D446" t="n">
+        <v>34</v>
+      </c>
+      <c r="E446" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>446</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>13:43:55</t>
+        </is>
+      </c>
+      <c r="D447" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E447" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>447</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>13:44:58</t>
+        </is>
+      </c>
+      <c r="D448" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E448" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>448</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>13:45:59</t>
+        </is>
+      </c>
+      <c r="D449" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E449" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>449</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>13:47:03</t>
+        </is>
+      </c>
+      <c r="D450" t="n">
+        <v>34</v>
+      </c>
+      <c r="E450" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>450</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>13:48:04</t>
+        </is>
+      </c>
+      <c r="D451" t="n">
+        <v>34</v>
+      </c>
+      <c r="E451" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>451</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>13:49:05</t>
+        </is>
+      </c>
+      <c r="D452" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E452" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>452</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>13:50:09</t>
+        </is>
+      </c>
+      <c r="D453" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E453" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>453</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>13:51:13</t>
+        </is>
+      </c>
+      <c r="D454" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E454" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>454</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>13:52:24</t>
+        </is>
+      </c>
+      <c r="D455" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="E455" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>455</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>13:53:27</t>
+        </is>
+      </c>
+      <c r="D456" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E456" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>456</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>13:54:15</t>
+        </is>
+      </c>
+      <c r="D457" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E457" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>457</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>13:55:35</t>
+        </is>
+      </c>
+      <c r="D458" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E458" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>458</v>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>14:06:15</t>
+        </is>
+      </c>
+      <c r="D459" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E459" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F459" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>459</v>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>14:07:37</t>
+        </is>
+      </c>
+      <c r="D460" t="n">
+        <v>34</v>
+      </c>
+      <c r="E460" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F460" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>460</v>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>14:08:42</t>
+        </is>
+      </c>
+      <c r="D461" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E461" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F461" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>461</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>14:09:46</t>
+        </is>
+      </c>
+      <c r="D462" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E462" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>462</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>14:10:49</t>
+        </is>
+      </c>
+      <c r="D463" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E463" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>463</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>14:11:53</t>
+        </is>
+      </c>
+      <c r="D464" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E464" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>464</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>14:12:54</t>
+        </is>
+      </c>
+      <c r="D465" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E465" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>465</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>14:14:01</t>
+        </is>
+      </c>
+      <c r="D466" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E466" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>466</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>14:15:31</t>
+        </is>
+      </c>
+      <c r="D467" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E467" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>467</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>14:19:54</t>
+        </is>
+      </c>
+      <c r="D468" t="n">
+        <v>34</v>
+      </c>
+      <c r="E468" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G468" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>468</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>14:20:30</t>
+        </is>
+      </c>
+      <c r="D469" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="E469" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>469</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>14:21:16</t>
+        </is>
+      </c>
+      <c r="D470" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="E470" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>470</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>14:22:26</t>
+        </is>
+      </c>
+      <c r="D471" t="n">
+        <v>34</v>
+      </c>
+      <c r="E471" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F471" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>471</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>14:23:27</t>
+        </is>
+      </c>
+      <c r="D472" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E472" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F472" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>472</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>14:24:31</t>
+        </is>
+      </c>
+      <c r="D473" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E473" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F473" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>473</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>14:25:47</t>
+        </is>
+      </c>
+      <c r="D474" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="E474" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>474</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>14:26:48</t>
+        </is>
+      </c>
+      <c r="D475" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E475" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F475" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>475</v>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>14:27:30</t>
+        </is>
+      </c>
+      <c r="D476" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E476" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>476</v>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>14:30:22</t>
+        </is>
+      </c>
+      <c r="D477" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E477" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F477" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>477</v>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>14:31:37</t>
+        </is>
+      </c>
+      <c r="D478" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E478" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F478" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>478</v>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>14:37:19</t>
+        </is>
+      </c>
+      <c r="D479" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E479" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F479" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>479</v>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>14:44:12</t>
+        </is>
+      </c>
+      <c r="D480" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E480" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F480" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>480</v>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>14:45:32</t>
+        </is>
+      </c>
+      <c r="D481" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E481" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>481</v>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>14:46:40</t>
+        </is>
+      </c>
+      <c r="D482" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E482" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F482" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>482</v>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>14:47:13</t>
+        </is>
+      </c>
+      <c r="D483" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E483" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="F483" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>483</v>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>14:48:37</t>
+        </is>
+      </c>
+      <c r="D484" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E484" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F484" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Last Run at Continental before Urlaub :)
</commit_message>
<xml_diff>
--- a/SensorMessungen.xlsx
+++ b/SensorMessungen.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G484"/>
+  <dimension ref="A1:G497"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15440,6 +15440,409 @@
         </is>
       </c>
     </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>484</v>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>14:49:43</t>
+        </is>
+      </c>
+      <c r="D485" t="n">
+        <v>34</v>
+      </c>
+      <c r="E485" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F485" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>485</v>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>14:50:45</t>
+        </is>
+      </c>
+      <c r="D486" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E486" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>486</v>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>14:51:48</t>
+        </is>
+      </c>
+      <c r="D487" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E487" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F487" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>487</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>14:52:49</t>
+        </is>
+      </c>
+      <c r="D488" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="E488" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>488</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>14:53:50</t>
+        </is>
+      </c>
+      <c r="D489" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E489" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F489" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>489</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>14:54:54</t>
+        </is>
+      </c>
+      <c r="D490" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E490" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F490" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>490</v>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>14:55:58</t>
+        </is>
+      </c>
+      <c r="D491" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E491" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F491" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>491</v>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>14:57:04</t>
+        </is>
+      </c>
+      <c r="D492" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="E492" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="F492" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>492</v>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>14:58:05</t>
+        </is>
+      </c>
+      <c r="D493" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E493" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="F493" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>493</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>14:59:06</t>
+        </is>
+      </c>
+      <c r="D494" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E494" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>494</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>15:00:07</t>
+        </is>
+      </c>
+      <c r="D495" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="E495" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>495</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>15:01:08</t>
+        </is>
+      </c>
+      <c r="D496" t="n">
+        <v>34</v>
+      </c>
+      <c r="E496" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>496</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>28.11.2023</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>15:05:56</t>
+        </is>
+      </c>
+      <c r="D497" t="n">
+        <v>34.8</v>
+      </c>
+      <c r="E497" t="n">
+        <v>21</v>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G497" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>